<commit_message>
AFR/Lambda & EGT in Recalc
</commit_message>
<xml_diff>
--- a/LabVIEW/99_Source/Recalc Offen.xlsx
+++ b/LabVIEW/99_Source/Recalc Offen.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Vespa-Prüfstand\WildBugChilGru\LabVIEW\99_Source\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58646E73-9C7B-4F85-A0BF-BA863CDC8EAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFBBAB95-9361-40CD-B74B-C13EBD696B84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="15750" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,9 +30,6 @@
     <t>Umschaltung AFR &lt;&gt; Lambda</t>
   </si>
   <si>
-    <t>Y-Achsen Skalierung ändern?</t>
-  </si>
-  <si>
     <t>Plot Farben:</t>
   </si>
   <si>
@@ -76,6 +73,9 @@
   </si>
   <si>
     <t>Plots anzeigen</t>
+  </si>
+  <si>
+    <t>Y-Achsen Skalierung ändern</t>
   </si>
 </sst>
 </file>
@@ -396,7 +396,7 @@
   <dimension ref="A1:A18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -406,7 +406,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
@@ -416,77 +416,77 @@
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>1</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>